<commit_message>
Add dual DataFrames for same-day transactions and correct totals
</commit_message>
<xml_diff>
--- a/excel/output_by_date.xlsx
+++ b/excel/output_by_date.xlsx
@@ -448,10 +448,10 @@
     <col width="16.3" customWidth="1" min="3" max="3"/>
     <col width="8.600000000000001" customWidth="1" min="4" max="4"/>
     <col width="21.8" customWidth="1" min="5" max="5"/>
-    <col width="21.8" customWidth="1" min="6" max="6"/>
+    <col width="18.5" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
-    <col width="8.600000000000001" customWidth="1" min="8" max="8"/>
-    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="16.3" customWidth="1" min="8" max="8"/>
+    <col width="17.4" customWidth="1" min="9" max="9"/>
     <col width="13" customWidth="1" min="10" max="10"/>
     <col width="10.8" customWidth="1" min="11" max="11"/>
     <col width="9.700000000000001" customWidth="1" min="12" max="12"/>
@@ -463,11 +463,11 @@
     <col width="16.3" customWidth="1" min="18" max="18"/>
     <col width="11.9" customWidth="1" min="19" max="19"/>
     <col width="14.1" customWidth="1" min="20" max="20"/>
-    <col width="9.700000000000001" customWidth="1" min="21" max="21"/>
+    <col width="16.3" customWidth="1" min="21" max="21"/>
     <col width="9.700000000000001" customWidth="1" min="22" max="22"/>
     <col width="13" customWidth="1" min="23" max="23"/>
     <col width="10.8" customWidth="1" min="24" max="24"/>
-    <col width="21.8" customWidth="1" min="25" max="25"/>
+    <col width="27.3" customWidth="1" min="25" max="25"/>
     <col width="11.9" customWidth="1" min="26" max="26"/>
     <col width="6.4" customWidth="1" min="27" max="27"/>
     <col width="8.600000000000001" customWidth="1" min="28" max="28"/>
@@ -489,8 +489,8 @@
     <col width="9.700000000000001" customWidth="1" min="44" max="44"/>
     <col width="15.2" customWidth="1" min="45" max="45"/>
     <col width="8.600000000000001" customWidth="1" min="46" max="46"/>
-    <col width="21.8" customWidth="1" min="47" max="47"/>
-    <col width="10.8" customWidth="1" min="48" max="48"/>
+    <col width="36.1" customWidth="1" min="47" max="47"/>
+    <col width="35" customWidth="1" min="48" max="48"/>
     <col width="13" customWidth="1" min="49" max="49"/>
     <col width="14.1" customWidth="1" min="50" max="50"/>
     <col width="13" customWidth="1" min="51" max="51"/>
@@ -498,7 +498,7 @@
     <col width="9.700000000000001" customWidth="1" min="53" max="53"/>
     <col width="14.1" customWidth="1" min="54" max="54"/>
     <col width="22.9" customWidth="1" min="55" max="55"/>
-    <col width="9.700000000000001" customWidth="1" min="56" max="56"/>
+    <col width="18.5" customWidth="1" min="56" max="56"/>
     <col width="7.5" customWidth="1" min="57" max="57"/>
     <col width="11.9" customWidth="1" min="58" max="58"/>
     <col width="10.8" customWidth="1" min="59" max="59"/>
@@ -900,8 +900,10 @@
       <c r="AP5" t="n">
         <v>-45</v>
       </c>
-      <c r="AU5" t="n">
-        <v>-11.32</v>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>-4.70 + -6.62</t>
+        </is>
       </c>
       <c r="BL5" t="n">
         <v>-9.74</v>
@@ -967,11 +969,15 @@
           <t>12-2-2024</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>-66.57000000000001</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>-25.45</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-25.30 + -41.27</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>-9.22 + -16.23</t>
+        </is>
       </c>
       <c r="AB12" t="n">
         <v>-7</v>
@@ -995,8 +1001,10 @@
           <t>12-3-2024</t>
         </is>
       </c>
-      <c r="H13" t="n">
-        <v>-7.52</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-0.93 + -6.59</t>
+        </is>
       </c>
       <c r="AW13" t="n">
         <v>-50</v>
@@ -1076,8 +1084,10 @@
       <c r="Q19" t="n">
         <v>-239.86</v>
       </c>
-      <c r="Y19" t="n">
-        <v>-39.03</v>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>-11.12 + -27.91</t>
+        </is>
       </c>
       <c r="AI19" t="n">
         <v>-31.18</v>
@@ -1164,8 +1174,10 @@
           <t>12-16-2024</t>
         </is>
       </c>
-      <c r="Y26" t="n">
-        <v>-59.98999999999999</v>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>-25.49 + -34.50</t>
+        </is>
       </c>
       <c r="AL26" t="n">
         <v>-20</v>
@@ -1217,8 +1229,10 @@
       <c r="AN28" t="n">
         <v>-85</v>
       </c>
-      <c r="AU28" t="n">
-        <v>-38.79</v>
+      <c r="AU28" t="inlineStr">
+        <is>
+          <t>-2.45 + -6.62 + -29.72</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1282,8 +1296,10 @@
       <c r="C33" t="n">
         <v>-13.19</v>
       </c>
-      <c r="M33" t="n">
-        <v>-12.89</v>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>-4.12 + -8.77</t>
+        </is>
       </c>
       <c r="O33" t="n">
         <v>-70</v>
@@ -1304,8 +1320,10 @@
           <t>12-24-2024</t>
         </is>
       </c>
-      <c r="I34" t="n">
-        <v>320</v>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>20.00 + 300.00</t>
+        </is>
       </c>
       <c r="J34" t="n">
         <v>-500</v>
@@ -1373,8 +1391,10 @@
       <c r="AP40" t="n">
         <v>-45</v>
       </c>
-      <c r="AV40" t="n">
-        <v>-37.72</v>
+      <c r="AV40" t="inlineStr">
+        <is>
+          <t>-2.11 + -3.66 + -31.95</t>
+        </is>
       </c>
       <c r="AZ40" t="n">
         <v>-24.12</v>
@@ -1524,8 +1544,10 @@
       <c r="Q50" t="n">
         <v>-273.04</v>
       </c>
-      <c r="AU50" t="n">
-        <v>-22.02</v>
+      <c r="AU50" t="inlineStr">
+        <is>
+          <t>-2.47 + -2.77 + -16.78</t>
+        </is>
       </c>
       <c r="BF50" t="n">
         <v>-3.17</v>
@@ -1552,8 +1574,10 @@
       <c r="AK51" t="n">
         <v>152.58</v>
       </c>
-      <c r="AU51" t="n">
-        <v>-5.59</v>
+      <c r="AU51" t="inlineStr">
+        <is>
+          <t>-2.36 + -3.23</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -1611,8 +1635,10 @@
       <c r="Y56" t="n">
         <v>-31.25</v>
       </c>
-      <c r="AU56" t="n">
-        <v>-9.82</v>
+      <c r="AU56" t="inlineStr">
+        <is>
+          <t>-3.20 + -6.62</t>
+        </is>
       </c>
       <c r="BI56" t="n">
         <v>-10.77</v>
@@ -1633,8 +1659,10 @@
       <c r="AM57" t="n">
         <v>-1401.5</v>
       </c>
-      <c r="AU57" t="n">
-        <v>-8.350000000000001</v>
+      <c r="AU57" t="inlineStr">
+        <is>
+          <t>-1.95 + -3.20 + -3.20</t>
+        </is>
       </c>
       <c r="BD57" t="n">
         <v>-21.19</v>
@@ -1791,17 +1819,23 @@
           <t>1-27-2025</t>
         </is>
       </c>
-      <c r="Y68" t="n">
-        <v>-41.93</v>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>-15.13 + -26.80</t>
+        </is>
       </c>
       <c r="AP68" t="n">
         <v>-45</v>
       </c>
-      <c r="AU68" t="n">
-        <v>-12.74</v>
-      </c>
-      <c r="BD68" t="n">
-        <v>-37.08</v>
+      <c r="AU68" t="inlineStr">
+        <is>
+          <t>-2.95 + -3.17 + -6.62</t>
+        </is>
+      </c>
+      <c r="BD68" t="inlineStr">
+        <is>
+          <t>-8.47 + -28.61</t>
+        </is>
       </c>
       <c r="BH68" t="n">
         <v>-33.31</v>
@@ -1888,8 +1922,10 @@
       <c r="L75" t="n">
         <v>-7.52</v>
       </c>
-      <c r="Y75" t="n">
-        <v>-43.36</v>
+      <c r="Y75" t="inlineStr">
+        <is>
+          <t>-17.60 + -25.76</t>
+        </is>
       </c>
       <c r="AB75" t="n">
         <v>-14</v>
@@ -1897,8 +1933,10 @@
       <c r="AP75" t="n">
         <v>-45</v>
       </c>
-      <c r="AU75" t="n">
-        <v>-38.94</v>
+      <c r="AU75" t="inlineStr">
+        <is>
+          <t>-6.62 + -32.32</t>
+        </is>
       </c>
       <c r="AZ75" t="n">
         <v>-24.2</v>
@@ -1948,8 +1986,10 @@
       <c r="I78" t="n">
         <v>300</v>
       </c>
-      <c r="AU78" t="n">
-        <v>-9.050000000000001</v>
+      <c r="AU78" t="inlineStr">
+        <is>
+          <t>-2.43 + -6.62</t>
+        </is>
       </c>
       <c r="BL78" t="n">
         <v>-6.56</v>
@@ -1967,11 +2007,15 @@
       <c r="Q79" t="n">
         <v>-393.02</v>
       </c>
-      <c r="U79" t="n">
-        <v>-3.98</v>
-      </c>
-      <c r="Y79" t="n">
-        <v>-25.94</v>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>-1.99 + -1.99</t>
+        </is>
+      </c>
+      <c r="Y79" t="inlineStr">
+        <is>
+          <t>-11.70 + -14.24</t>
+        </is>
       </c>
       <c r="AK79" t="n">
         <v>417.13</v>
@@ -2021,11 +2065,15 @@
       <c r="AP82" t="n">
         <v>-45</v>
       </c>
-      <c r="AU82" t="n">
-        <v>-64.46000000000001</v>
-      </c>
-      <c r="BD82" t="n">
-        <v>-66.87</v>
+      <c r="AU82" t="inlineStr">
+        <is>
+          <t>-31.75 + -32.71</t>
+        </is>
+      </c>
+      <c r="BD82" t="inlineStr">
+        <is>
+          <t>-24.48 + -42.39</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -2113,8 +2161,10 @@
       <c r="T90" t="n">
         <v>-6</v>
       </c>
-      <c r="Y90" t="n">
-        <v>-107.05</v>
+      <c r="Y90" t="inlineStr">
+        <is>
+          <t>-6.00 + -23.93 + -77.12</t>
+        </is>
       </c>
       <c r="AG90" t="n">
         <v>-7.48</v>
@@ -2125,8 +2175,10 @@
       <c r="AP90" t="n">
         <v>-45</v>
       </c>
-      <c r="AU90" t="n">
-        <v>-30.08</v>
+      <c r="AU90" t="inlineStr">
+        <is>
+          <t>-4.76 + -25.32</t>
+        </is>
       </c>
       <c r="AV90" t="n">
         <v>-4.77</v>
@@ -2169,8 +2221,10 @@
           <t>2-20-2025</t>
         </is>
       </c>
-      <c r="AU92" t="n">
-        <v>-27.68</v>
+      <c r="AU92" t="inlineStr">
+        <is>
+          <t>-6.62 + -21.06</t>
+        </is>
       </c>
     </row>
     <row r="93">
@@ -2212,8 +2266,10 @@
       <c r="F96" t="n">
         <v>-60.99</v>
       </c>
-      <c r="M96" t="n">
-        <v>-12.43</v>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>-4.12 + -8.31</t>
+        </is>
       </c>
       <c r="AJ96" t="n">
         <v>-11.86</v>
@@ -2324,14 +2380,18 @@
       <c r="AU103" t="n">
         <v>-3.2</v>
       </c>
-      <c r="AV103" t="n">
-        <v>-44.74</v>
+      <c r="AV103" t="inlineStr">
+        <is>
+          <t>-2.99 + -3.56 + -3.56 + -34.63</t>
+        </is>
       </c>
       <c r="BB103" t="n">
         <v>-57</v>
       </c>
-      <c r="BD103" t="n">
-        <v>-22.95</v>
+      <c r="BD103" t="inlineStr">
+        <is>
+          <t>-7.06 + -15.89</t>
+        </is>
       </c>
       <c r="BE103" t="n">
         <v>-21.2</v>
@@ -2427,8 +2487,10 @@
       <c r="AP110" t="n">
         <v>-45</v>
       </c>
-      <c r="AU110" t="n">
-        <v>-27.58</v>
+      <c r="AU110" t="inlineStr">
+        <is>
+          <t>-3.20 + -24.38</t>
+        </is>
       </c>
       <c r="AZ110" t="n">
         <v>-46.35</v>
@@ -2527,8 +2589,10 @@
       <c r="AP117" t="n">
         <v>-45</v>
       </c>
-      <c r="AU117" t="n">
-        <v>-33.35</v>
+      <c r="AU117" t="inlineStr">
+        <is>
+          <t>-3.17 + -30.18</t>
+        </is>
       </c>
       <c r="AZ117" t="n">
         <v>-26.71</v>
@@ -2606,8 +2670,10 @@
       <c r="AK121" t="n">
         <v>1083</v>
       </c>
-      <c r="AU121" t="n">
-        <v>-74.27</v>
+      <c r="AU121" t="inlineStr">
+        <is>
+          <t>-30.13 + -31.38 + -9.59 + -3.17</t>
+        </is>
       </c>
       <c r="BL121" t="n">
         <v>-6.56</v>
@@ -2755,7 +2821,7 @@
         <v>-9.98</v>
       </c>
       <c r="AU122" s="2" t="n">
-        <v>-618.1399999999999</v>
+        <v>-618.14</v>
       </c>
       <c r="AV122" s="2" t="n">
         <v>-153.09</v>

</xml_diff>